<commit_message>
Commit before major changes
I've done a bunch of stuff and haven't committed in a while. I'm about to do a major reorganization of my repos, so this is to save everything before I break it.
</commit_message>
<xml_diff>
--- a/data-raw/Gtseq.val.locus.notes.xlsx
+++ b/data-raw/Gtseq.val.locus.notes.xlsx
@@ -1,122 +1,90 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shared/KKMDocuments/Documents/Github.Repos/Mnov/SNP-filtering-package/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BACDD1-C067-CC4B-9BA0-CDEEE75AB7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD67C02-E9C7-6149-85CB-2EC418AE2940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31080" yWindow="8280" windowWidth="27640" windowHeight="16940" xr2:uid="{9C1D80DB-9FB9-E84B-9564-A45792FDE54B}"/>
+    <workbookView xWindow="18380" yWindow="13840" windowWidth="27860" windowHeight="12280" xr2:uid="{9C1D80DB-9FB9-E84B-9564-A45792FDE54B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
-  <si>
-    <t>Mnov_gtseq_103</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Mnov_gtseq_155</t>
   </si>
   <si>
-    <t>Mnov_gtseq_188</t>
-  </si>
-  <si>
     <t>Mnov_gtseq_219</t>
   </si>
   <si>
-    <t>Mnov_gtseq_236</t>
-  </si>
-  <si>
-    <t>Mnov_gtseq_267</t>
-  </si>
-  <si>
     <t>Mnov_gtseq_302</t>
   </si>
   <si>
-    <t>Mnov_gtseq_304</t>
-  </si>
-  <si>
-    <t>Mnov_gtseq_330</t>
-  </si>
-  <si>
-    <t>Mnov_gtseq_367</t>
-  </si>
-  <si>
-    <t>Mnov_gtseq_382</t>
-  </si>
-  <si>
-    <t>Mnov_gtseq_417</t>
-  </si>
-  <si>
-    <t>Mnov_gtseq_431</t>
-  </si>
-  <si>
-    <t>Mnov_gtseq_551</t>
-  </si>
-  <si>
     <t>locus</t>
   </si>
   <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>This primer seems to be amplified a different target than intended</t>
-  </si>
-  <si>
-    <t>9 samples have &gt;2 haplotypes</t>
-  </si>
-  <si>
     <t>This should be recoverable - lots of Ns due to masked reads</t>
   </si>
   <si>
-    <t>Fine once I get rid of low coverage samples</t>
-  </si>
-  <si>
-    <t>A mess in all samples; drop</t>
-  </si>
-  <si>
     <t>There's a problem with the reverse primer; maybe can use forward reads only, but there might be an analogous locus being amplified</t>
   </si>
   <si>
-    <t>This is amplifying two different products - drop</t>
-  </si>
-  <si>
-    <t>This primer seems to be amplified a different target than intended and taking up a LOT of reads</t>
-  </si>
-  <si>
     <t>??</t>
   </si>
   <si>
     <t>Keep or Drop</t>
   </si>
   <si>
-    <t>Reject</t>
-  </si>
-  <si>
-    <t>Accept</t>
+    <t>Mnov_gtseq_541</t>
+  </si>
+  <si>
+    <t>This is amplifying two different products in non-humpbacks</t>
+  </si>
+  <si>
+    <t>Mnov_gtseq_535</t>
+  </si>
+  <si>
+    <t>The reverse primer produced 28,188 reads of something not the target!!!</t>
+  </si>
+  <si>
+    <t>Mnov_gtseq_420</t>
+  </si>
+  <si>
+    <t>This has almost no reads for a well-performing sample; check in rest of samples</t>
+  </si>
+  <si>
+    <t>Mnov_gtseq_110</t>
+  </si>
+  <si>
+    <t>This is generally messy. It's amplifying two different products - the target (90bp) and a 127 bp off-target read</t>
+  </si>
+  <si>
+    <t>This locus probably has 3 good SNPs, but microhaplot is calling 5; might be recoverable</t>
+  </si>
+  <si>
+    <t>Mnov_gtseq_474</t>
+  </si>
+  <si>
+    <t>This is messy and the vcf has waaaaayyyyy too many variants; might be recoverable if I figure out which sites are reliable SNPs</t>
   </si>
 </sst>
 </file>
@@ -468,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1249B02D-8D2F-7243-A4EC-4F2FE63C8321}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,170 +450,92 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C9">
+    <sortCondition ref="A2:A9"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>